<commit_message>
graphs for the paper
</commit_message>
<xml_diff>
--- a/results/ContrastBasedAttack.xlsx
+++ b/results/ContrastBasedAttack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\bandlimited-cnns\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BD2E9F-6438-487E-90C7-60E68AC413BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBA68A2-8C5F-489E-AFB8-2B71B1C29CA0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" activeTab="3" xr2:uid="{260C2C63-8E7C-4988-B91E-4EB3FB39E384}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" xr2:uid="{260C2C63-8E7C-4988-B91E-4EB3FB39E384}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="73">
   <si>
     <t>ssh://ady@skr-compute1.cs.uchicago.edu:22/home/ady/anaconda3/bin/python3.6 -u /home/ady/code/bandlimited-cnns/cnns/nnlib/pytorch_experiments/robustness/pytorch_resnet18_full_cifar10_attack.py</t>
   </si>
@@ -1804,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D7D62A-35BE-4F3F-84EA-35EC4BB02693}">
-  <dimension ref="A1:G215"/>
+  <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="K173" sqref="K173"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="E185" sqref="E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4614,26 +4614,26 @@
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A185">
-        <v>84</v>
+      <c r="A185" t="s">
+        <v>7</v>
       </c>
       <c r="B185" t="s">
-        <v>45</v>
-      </c>
-      <c r="C185">
-        <v>3.1</v>
-      </c>
-      <c r="D185">
-        <v>211</v>
-      </c>
-      <c r="E185">
-        <v>1000</v>
-      </c>
-      <c r="F185">
-        <v>0.21099999999999999</v>
-      </c>
-      <c r="G185">
-        <v>213.83094930648801</v>
+        <v>8</v>
+      </c>
+      <c r="C185" t="s">
+        <v>9</v>
+      </c>
+      <c r="D185" t="s">
+        <v>10</v>
+      </c>
+      <c r="E185" t="s">
+        <v>11</v>
+      </c>
+      <c r="F185" t="s">
+        <v>12</v>
+      </c>
+      <c r="G185" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4644,19 +4644,19 @@
         <v>45</v>
       </c>
       <c r="C186">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="D186">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E186">
         <v>1000</v>
       </c>
       <c r="F186">
-        <v>0.20699999999999999</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="G186">
-        <v>213.574878454208</v>
+        <v>213.83094930648801</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4667,19 +4667,19 @@
         <v>45</v>
       </c>
       <c r="C187">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="D187">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E187">
         <v>1000</v>
       </c>
       <c r="F187">
-        <v>0.20200000000000001</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="G187">
-        <v>218.57027316093399</v>
+        <v>213.574878454208</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4690,19 +4690,19 @@
         <v>45</v>
       </c>
       <c r="C188">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="D188">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E188">
         <v>1000</v>
       </c>
       <c r="F188">
-        <v>0.2</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="G188">
-        <v>175.267798185348</v>
+        <v>218.57027316093399</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4713,19 +4713,19 @@
         <v>45</v>
       </c>
       <c r="C189">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="D189">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E189">
         <v>1000</v>
       </c>
       <c r="F189">
-        <v>0.19600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G189">
-        <v>114.028005599975</v>
+        <v>175.267798185348</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4736,19 +4736,19 @@
         <v>45</v>
       </c>
       <c r="C190">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="D190">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E190">
         <v>1000</v>
       </c>
       <c r="F190">
-        <v>0.20100000000000001</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="G190">
-        <v>110.810024738311</v>
+        <v>114.028005599975</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4759,19 +4759,19 @@
         <v>45</v>
       </c>
       <c r="C191">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="D191">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="E191">
         <v>1000</v>
       </c>
       <c r="F191">
-        <v>0.19700000000000001</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="G191">
-        <v>116.037495613098</v>
+        <v>110.810024738311</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4782,19 +4782,19 @@
         <v>45</v>
       </c>
       <c r="C192">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="D192">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E192">
         <v>1000</v>
       </c>
       <c r="F192">
-        <v>0.193</v>
+        <v>0.19700000000000001</v>
       </c>
       <c r="G192">
-        <v>110.18922114372199</v>
+        <v>116.037495613098</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4805,19 +4805,19 @@
         <v>45</v>
       </c>
       <c r="C193">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="D193">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E193">
         <v>1000</v>
       </c>
       <c r="F193">
-        <v>0.185</v>
+        <v>0.193</v>
       </c>
       <c r="G193">
-        <v>109.601399421691</v>
+        <v>110.18922114372199</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4828,47 +4828,47 @@
         <v>45</v>
       </c>
       <c r="C194">
+        <v>3.9</v>
+      </c>
+      <c r="D194">
+        <v>185</v>
+      </c>
+      <c r="E194">
+        <v>1000</v>
+      </c>
+      <c r="F194">
+        <v>0.185</v>
+      </c>
+      <c r="G194">
+        <v>109.601399421691</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195">
+        <v>84</v>
+      </c>
+      <c r="B195" t="s">
+        <v>45</v>
+      </c>
+      <c r="C195">
         <v>4</v>
       </c>
-      <c r="D194">
+      <c r="D195">
         <v>184</v>
       </c>
-      <c r="E194">
-        <v>1000</v>
-      </c>
-      <c r="F194">
+      <c r="E195">
+        <v>1000</v>
+      </c>
+      <c r="F195">
         <v>0.184</v>
       </c>
-      <c r="G194">
+      <c r="G195">
         <v>108.762120723724</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A195" t="s">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A196">
-        <v>0</v>
-      </c>
-      <c r="B196" t="s">
-        <v>45</v>
-      </c>
-      <c r="C196">
-        <v>3.1</v>
-      </c>
-      <c r="D196">
-        <v>385</v>
-      </c>
-      <c r="E196">
-        <v>1000</v>
-      </c>
-      <c r="F196">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="G196">
-        <v>131.641612052917</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4879,34 +4879,52 @@
         <v>45</v>
       </c>
       <c r="C197">
+        <v>3.1</v>
+      </c>
+      <c r="D197">
+        <v>385</v>
+      </c>
+      <c r="E197">
+        <v>1000</v>
+      </c>
+      <c r="F197">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="G197">
+        <v>131.641612052917</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198">
+        <v>0</v>
+      </c>
+      <c r="B198" t="s">
+        <v>45</v>
+      </c>
+      <c r="C198">
         <v>3.2</v>
       </c>
-      <c r="D197">
+      <c r="D198">
         <v>382</v>
       </c>
-      <c r="E197">
-        <v>1000</v>
-      </c>
-      <c r="F197">
+      <c r="E198">
+        <v>1000</v>
+      </c>
+      <c r="F198">
         <v>0.38200000000000001</v>
       </c>
-      <c r="G197">
+      <c r="G198">
         <v>133.40115904807999</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A199" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4916,68 +4934,50 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" t="s">
-        <v>7</v>
-      </c>
-      <c r="B205" t="s">
-        <v>8</v>
-      </c>
-      <c r="C205" t="s">
-        <v>9</v>
-      </c>
-      <c r="D205" t="s">
-        <v>10</v>
-      </c>
-      <c r="E205" t="s">
-        <v>11</v>
-      </c>
-      <c r="F205" t="s">
-        <v>12</v>
-      </c>
-      <c r="G205" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" t="s">
-        <v>47</v>
+        <v>7</v>
+      </c>
+      <c r="B206" t="s">
+        <v>8</v>
+      </c>
+      <c r="C206" t="s">
+        <v>9</v>
+      </c>
+      <c r="D206" t="s">
+        <v>10</v>
+      </c>
+      <c r="E206" t="s">
+        <v>11</v>
+      </c>
+      <c r="F206" t="s">
+        <v>12</v>
+      </c>
+      <c r="G206" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A208">
-        <v>0</v>
-      </c>
-      <c r="B208" t="s">
-        <v>45</v>
-      </c>
-      <c r="C208">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D208">
-        <v>307</v>
-      </c>
-      <c r="E208">
-        <v>1000</v>
-      </c>
-      <c r="F208">
-        <v>0.307</v>
-      </c>
-      <c r="G208">
-        <v>132.52118659019399</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4988,19 +4988,19 @@
         <v>45</v>
       </c>
       <c r="C209">
-        <v>4.1999999999999904</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D209">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="E209">
         <v>1000</v>
       </c>
       <c r="F209">
-        <v>0.3</v>
+        <v>0.307</v>
       </c>
       <c r="G209">
-        <v>128.12920522689799</v>
+        <v>132.52118659019399</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5011,19 +5011,19 @@
         <v>45</v>
       </c>
       <c r="C210">
-        <v>4.3</v>
+        <v>4.1999999999999904</v>
       </c>
       <c r="D210">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="E210">
         <v>1000</v>
       </c>
       <c r="F210">
-        <v>0.29699999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="G210">
-        <v>134.34096002578701</v>
+        <v>128.12920522689799</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5034,19 +5034,19 @@
         <v>45</v>
       </c>
       <c r="C211">
-        <v>4.3999999999999897</v>
+        <v>4.3</v>
       </c>
       <c r="D211">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="E211">
         <v>1000</v>
       </c>
       <c r="F211">
-        <v>0.29199999999999998</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="G211">
-        <v>134.158747434616</v>
+        <v>134.34096002578701</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5057,19 +5057,19 @@
         <v>45</v>
       </c>
       <c r="C212">
-        <v>4.5</v>
+        <v>4.3999999999999897</v>
       </c>
       <c r="D212">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="E212">
         <v>1000</v>
       </c>
       <c r="F212">
-        <v>0.28699999999999998</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="G212">
-        <v>129.995982646942</v>
+        <v>134.158747434616</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5080,19 +5080,19 @@
         <v>45</v>
       </c>
       <c r="C213">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="D213">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="E213">
         <v>1000</v>
       </c>
       <c r="F213">
-        <v>0.28000000000000003</v>
+        <v>0.28699999999999998</v>
       </c>
       <c r="G213">
-        <v>128.85620260238599</v>
+        <v>129.995982646942</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5103,19 +5103,19 @@
         <v>45</v>
       </c>
       <c r="C214">
-        <v>4.6999999999999904</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D214">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="E214">
         <v>1000</v>
       </c>
       <c r="F214">
-        <v>0.27200000000000002</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G214">
-        <v>128.19307279586701</v>
+        <v>128.85620260238599</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5126,18 +5126,41 @@
         <v>45</v>
       </c>
       <c r="C215">
+        <v>4.6999999999999904</v>
+      </c>
+      <c r="D215">
+        <v>272</v>
+      </c>
+      <c r="E215">
+        <v>1000</v>
+      </c>
+      <c r="F215">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G215">
+        <v>128.19307279586701</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A216">
+        <v>0</v>
+      </c>
+      <c r="B216" t="s">
+        <v>45</v>
+      </c>
+      <c r="C216">
         <v>4.8</v>
       </c>
-      <c r="D215">
+      <c r="D216">
         <v>271</v>
       </c>
-      <c r="E215">
-        <v>1000</v>
-      </c>
-      <c r="F215">
+      <c r="E216">
+        <v>1000</v>
+      </c>
+      <c r="F216">
         <v>0.27100000000000002</v>
       </c>
-      <c r="G215">
+      <c r="G216">
         <v>133.701603412628</v>
       </c>
     </row>
@@ -5153,7 +5176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944858AC-1F24-4928-A268-B44DE54D1291}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -5582,7 +5605,7 @@
         <v>3.1</v>
       </c>
       <c r="B33">
-        <f>data!F196*100</f>
+        <f>data!F197*100</f>
         <v>38.5</v>
       </c>
       <c r="C33">
@@ -5599,7 +5622,7 @@
         <v>38.200000000000003</v>
       </c>
       <c r="C34">
-        <f>data!F186*100</f>
+        <f>data!F187*100</f>
         <v>20.7</v>
       </c>
     </row>
@@ -5612,7 +5635,7 @@
         <v>37.299999999999997</v>
       </c>
       <c r="C35">
-        <f>data!F187*100</f>
+        <f>data!F188*100</f>
         <v>20.200000000000003</v>
       </c>
     </row>
@@ -5625,7 +5648,7 @@
         <v>36.700000000000003</v>
       </c>
       <c r="C36">
-        <f>data!F188*100</f>
+        <f>data!F189*100</f>
         <v>20</v>
       </c>
     </row>
@@ -5638,7 +5661,7 @@
         <v>35.699999999999996</v>
       </c>
       <c r="C37">
-        <f>data!F189*100</f>
+        <f>data!F190*100</f>
         <v>19.600000000000001</v>
       </c>
     </row>
@@ -5651,7 +5674,7 @@
         <v>35.099999999999994</v>
       </c>
       <c r="C38">
-        <f>data!F190*100</f>
+        <f>data!F191*100</f>
         <v>20.100000000000001</v>
       </c>
     </row>
@@ -5664,7 +5687,7 @@
         <v>34</v>
       </c>
       <c r="C39">
-        <f>data!F191*100</f>
+        <f>data!F192*100</f>
         <v>19.7</v>
       </c>
     </row>
@@ -5677,7 +5700,7 @@
         <v>33.4</v>
       </c>
       <c r="C40">
-        <f>data!F192*100</f>
+        <f>data!F193*100</f>
         <v>19.3</v>
       </c>
     </row>
@@ -5690,7 +5713,7 @@
         <v>32.700000000000003</v>
       </c>
       <c r="C41">
-        <f>data!F193*100</f>
+        <f>data!F194*100</f>
         <v>18.5</v>
       </c>
     </row>
@@ -5703,7 +5726,7 @@
         <v>31.6</v>
       </c>
       <c r="C42">
-        <f>data!F194*100</f>
+        <f>data!F195*100</f>
         <v>18.399999999999999</v>
       </c>
     </row>
@@ -5712,7 +5735,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B43">
-        <f>data!F208*100</f>
+        <f>data!F209*100</f>
         <v>30.7</v>
       </c>
     </row>
@@ -5721,7 +5744,7 @@
         <v>4.2</v>
       </c>
       <c r="B44">
-        <f>data!F209*100</f>
+        <f>data!F210*100</f>
         <v>30</v>
       </c>
     </row>
@@ -5730,7 +5753,7 @@
         <v>4.3</v>
       </c>
       <c r="B45">
-        <f>data!F210*100</f>
+        <f>data!F211*100</f>
         <v>29.7</v>
       </c>
     </row>
@@ -5739,7 +5762,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B46">
-        <f>data!F211*100</f>
+        <f>data!F212*100</f>
         <v>29.2</v>
       </c>
     </row>
@@ -5748,7 +5771,7 @@
         <v>4.5</v>
       </c>
       <c r="B47">
-        <f>data!F212*100</f>
+        <f>data!F213*100</f>
         <v>28.7</v>
       </c>
     </row>
@@ -5757,7 +5780,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="B48">
-        <f>data!F213*100</f>
+        <f>data!F214*100</f>
         <v>28.000000000000004</v>
       </c>
     </row>
@@ -5766,7 +5789,7 @@
         <v>4.7</v>
       </c>
       <c r="B49">
-        <f>data!F214*100</f>
+        <f>data!F215*100</f>
         <v>27.200000000000003</v>
       </c>
     </row>
@@ -5797,7 +5820,7 @@
   <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="L61" sqref="L61:L72"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7415,7 +7438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051C7734-AEE3-4908-96A6-2FF5389E06C1}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>

</xml_diff>